<commit_message>
sheets de control ahora con id y nombre
actualizado para inclir id de los giros y las ocupaciones, dos columnas en el sheet giros, 4 columnas en el sheet de ocupaciones
</commit_message>
<xml_diff>
--- a/venv/master_template.xlsx
+++ b/venv/master_template.xlsx
@@ -862,7 +862,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19"/>
@@ -2882,12 +2882,12 @@
       <formula1>$giro.$a</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C1001" type="list">
-      <formula1>Giro!$A:$A</formula1>
+    <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D1001" type="list">
+      <formula1>OFFSET(Ocupacion!$D$1, MATCH(C2,Ocupacion!$B:$B,0)-1, 0, COUNTIF(Ocupacion!$B:$B,C2), 1)</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D1001" type="list">
-      <formula1>OFFSET(Ocupacion!$B$1, MATCH(C2,Ocupacion!$A:$A,0)-1, 0, COUNTIF(Ocupacion!$A:$A,C2), 1)</formula1>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C1001" type="list">
+      <formula1>Giro!$B:$B</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -2909,10 +2909,10 @@
   <dimension ref="A1:AB201"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19"/>
@@ -4942,7 +4942,7 @@
       <c r="J201" s="11"/>
     </row>
   </sheetData>
-  <dataValidations count="5">
+  <dataValidations count="4">
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="N2:N31" type="list">
       <formula1>Cuestionario</formula1>
       <formula2>0</formula2>
@@ -4951,16 +4951,12 @@
       <formula1>Estados!$A$1:$A$26</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C1001" type="list">
-      <formula1>Giro!$A:$A</formula1>
+    <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D1001" type="list">
+      <formula1>OFFSET(Ocupacion!$D$1, MATCH(C2,Ocupacion!$B:$B,0)-1, 0, COUNTIF(Ocupacion!$B:$B,C2), 1)</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D4 D6:D1001" type="list">
-      <formula1>OFFSET(Ocupacion!$B$1, MATCH(C2,Ocupacion!$A:$A,0)-1, 0, COUNTIF(Ocupacion!$A:$A,C2), 1)</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D5" type="list">
-      <formula1>OFFSET(Ocupacion!$B$1, MATCH(C5,Ocupacion!$A:$A,0)-1, 0, COUNTIF(Ocupacion!$A:$A,C5), 1)</formula1>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C1001" type="list">
+      <formula1>Giro!$B:$B</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -5426,7 +5422,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.734375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.37"/>
@@ -5665,146 +5661,16 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A131" activeCellId="0" sqref="A131"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="40.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="8.36"/>
   </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-  </sheetData>
+  <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -5826,7 +5692,7 @@
       <selection pane="topLeft" activeCell="B2678" activeCellId="0" sqref="B2678"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.734375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="56.87"/>

</xml_diff>